<commit_message>
inanc beoordeling and blog
</commit_message>
<xml_diff>
--- a/persoonlijk beoordelling/inanc/Project5 Beoordeling.xlsx
+++ b/persoonlijk beoordelling/inanc/Project5 Beoordeling.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inanc\Desktop\school\leerjaar 2\Project 5\SummaMove\beoordelling\inanc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quinc\Documents\Dev\School\Jaar 2\Projecten\Project 5\Git\SummaMove\persoonlijk beoordelling\inanc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33802DC9-D033-4FA5-8E86-384F4A5D903D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF06F8E0-3F0D-407A-85D0-A5FECB06BBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad2" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="92">
   <si>
     <t>Groep1</t>
   </si>
@@ -851,37 +851,37 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G28" sqref="G28"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="46.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="3.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="46.1796875" style="2" customWidth="1"/>
     <col min="4" max="4" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="3.5703125" style="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="16384" width="8.85546875" style="1"/>
+    <col min="5" max="7" width="3.54296875" style="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="4"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C3" s="4"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -898,7 +898,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="5" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -908,14 +908,14 @@
       </c>
       <c r="F5" s="8" t="str">
         <f>IF(COUNTIF(F6:F12,"v")=7,"V","O")</f>
-        <v>O</v>
+        <v>V</v>
       </c>
       <c r="G5" s="8" t="str">
         <f>IF(COUNTIF(G6:G12,"v")=7,"V","O")</f>
         <v>V</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="29" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
@@ -929,7 +929,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
@@ -943,7 +943,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="29" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
@@ -957,19 +957,21 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="29" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>88</v>
+      </c>
       <c r="G9" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="45" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="43.5" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
@@ -983,7 +985,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C11" s="2" t="s">
         <v>8</v>
       </c>
@@ -997,7 +999,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="43.5" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1011,7 +1013,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
@@ -1028,7 +1030,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="14" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
@@ -1045,7 +1047,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
@@ -1062,7 +1064,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C16" s="2" t="s">
         <v>13</v>
       </c>
@@ -1079,7 +1081,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="17" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1096,7 +1098,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="18" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C18" s="2" t="s">
         <v>15</v>
       </c>
@@ -1113,7 +1115,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="19" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C19" s="2" t="s">
         <v>16</v>
       </c>
@@ -1130,7 +1132,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
@@ -1147,7 +1149,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="21" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C21" s="2" t="s">
         <v>18</v>
       </c>
@@ -1164,7 +1166,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="22" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C22" s="2" t="s">
         <v>19</v>
       </c>
@@ -1181,12 +1183,12 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -1203,7 +1205,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="27" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B27" s="1" t="s">
         <v>22</v>
       </c>
@@ -1220,7 +1222,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="28" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C28" s="2" t="s">
         <v>23</v>
       </c>
@@ -1228,7 +1230,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C29" s="2" t="s">
         <v>24</v>
       </c>
@@ -1236,7 +1238,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C30" s="2" t="s">
         <v>25</v>
       </c>
@@ -1244,7 +1246,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
         <v>26</v>
       </c>
@@ -1252,7 +1254,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
     </row>
-    <row r="32" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B32" s="1" t="s">
         <v>27</v>
       </c>
@@ -1260,7 +1262,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B33" s="1" t="s">
         <v>28</v>
       </c>
@@ -1268,7 +1270,7 @@
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B34" s="1" t="s">
         <v>29</v>
       </c>
@@ -1276,7 +1278,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B35" s="1" t="s">
         <v>30</v>
       </c>
@@ -1284,7 +1286,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B36" s="1" t="s">
         <v>31</v>
       </c>
@@ -1292,7 +1294,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B37" s="1" t="s">
         <v>32</v>
       </c>
@@ -1300,7 +1302,7 @@
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>33</v>
       </c>
@@ -1317,7 +1319,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="39" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="B39" s="1" t="s">
         <v>34</v>
       </c>
@@ -1325,7 +1327,7 @@
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="B40" s="1" t="s">
         <v>35</v>
       </c>
@@ -1333,7 +1335,7 @@
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="B41" s="1" t="s">
         <v>36</v>
       </c>
@@ -1341,7 +1343,7 @@
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>37</v>
       </c>
@@ -1358,7 +1360,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="44" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B44" s="1" t="s">
         <v>38</v>
       </c>
@@ -1375,7 +1377,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="45" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C45" s="2" t="s">
         <v>39</v>
       </c>
@@ -1383,7 +1385,7 @@
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C46" s="2" t="s">
         <v>40</v>
       </c>
@@ -1391,7 +1393,7 @@
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="B47" s="1" t="s">
         <v>41</v>
       </c>
@@ -1399,7 +1401,7 @@
       <c r="F47" s="7"/>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="B48" s="1" t="s">
         <v>42</v>
       </c>
@@ -1407,12 +1409,12 @@
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
     </row>
-    <row r="49" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B49" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>44</v>
       </c>
@@ -1429,7 +1431,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B52" s="1" t="s">
         <v>45</v>
       </c>
@@ -1437,7 +1439,7 @@
       <c r="F52" s="7"/>
       <c r="G52" s="7"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B53" s="1" t="s">
         <v>46</v>
       </c>
@@ -1445,12 +1447,12 @@
       <c r="F53" s="7"/>
       <c r="G53" s="7"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>48</v>
       </c>
@@ -1467,7 +1469,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="57" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B57" s="1" t="s">
         <v>49</v>
       </c>
@@ -1475,17 +1477,17 @@
       <c r="F57" s="7"/>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C58" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B59" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C60" s="2" t="s">
         <v>52</v>
       </c>
@@ -1493,7 +1495,7 @@
       <c r="F60" s="7"/>
       <c r="G60" s="7"/>
     </row>
-    <row r="61" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="29" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C61" s="2" t="s">
         <v>53</v>
       </c>
@@ -1501,7 +1503,7 @@
       <c r="F61" s="7"/>
       <c r="G61" s="7"/>
     </row>
-    <row r="62" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C62" s="2" t="s">
         <v>54</v>
       </c>
@@ -1509,12 +1511,12 @@
       <c r="F62" s="7"/>
       <c r="G62" s="7"/>
     </row>
-    <row r="63" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B63" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C64" s="2" t="s">
         <v>56</v>
       </c>
@@ -1522,7 +1524,7 @@
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
     </row>
-    <row r="65" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C65" s="2" t="s">
         <v>57</v>
       </c>
@@ -1530,7 +1532,7 @@
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
     </row>
-    <row r="66" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B66" s="1" t="s">
         <v>58</v>
       </c>
@@ -1538,7 +1540,7 @@
       <c r="F66" s="7"/>
       <c r="G66" s="7"/>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>59</v>
       </c>
@@ -1555,7 +1557,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="68" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B68" s="1" t="s">
         <v>60</v>
       </c>
@@ -1563,12 +1565,12 @@
       <c r="F68" s="7"/>
       <c r="G68" s="7"/>
     </row>
-    <row r="69" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="29" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C69" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="70" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B70" s="1" t="s">
         <v>62</v>
       </c>
@@ -1576,7 +1578,7 @@
       <c r="F70" s="7"/>
       <c r="G70" s="7"/>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>63</v>
       </c>
@@ -1593,7 +1595,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="73" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B73" s="1" t="s">
         <v>64</v>
       </c>
@@ -1601,7 +1603,7 @@
       <c r="F73" s="7"/>
       <c r="G73" s="7"/>
     </row>
-    <row r="74" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B74" s="1" t="s">
         <v>65</v>
       </c>
@@ -1609,7 +1611,7 @@
       <c r="F74" s="7"/>
       <c r="G74" s="7"/>
     </row>
-    <row r="75" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B75" s="1" t="s">
         <v>66</v>
       </c>
@@ -1617,7 +1619,7 @@
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
     </row>
-    <row r="76" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B76" s="1" t="s">
         <v>67</v>
       </c>
@@ -1625,7 +1627,7 @@
       <c r="F76" s="7"/>
       <c r="G76" s="7"/>
     </row>
-    <row r="77" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B77" s="1" t="s">
         <v>68</v>
       </c>
@@ -1633,7 +1635,7 @@
       <c r="F77" s="7"/>
       <c r="G77" s="7"/>
     </row>
-    <row r="78" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B78" s="1" t="s">
         <v>69</v>
       </c>
@@ -1641,7 +1643,7 @@
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>70</v>
       </c>
@@ -1658,7 +1660,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="80" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B80" s="1" t="s">
         <v>71</v>
       </c>
@@ -1666,7 +1668,7 @@
       <c r="F80" s="7"/>
       <c r="G80" s="7"/>
     </row>
-    <row r="81" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B81" s="1" t="s">
         <v>72</v>
       </c>
@@ -1674,12 +1676,12 @@
       <c r="F81" s="7"/>
       <c r="G81" s="7"/>
     </row>
-    <row r="82" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B82" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="29" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C83" s="2" t="s">
         <v>73</v>
       </c>
@@ -1687,7 +1689,7 @@
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
     </row>
-    <row r="84" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="29" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C84" s="2" t="s">
         <v>74</v>
       </c>
@@ -1695,7 +1697,7 @@
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
     </row>
-    <row r="85" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="29" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C85" s="2" t="s">
         <v>74</v>
       </c>
@@ -1703,12 +1705,12 @@
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
     </row>
-    <row r="86" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B86" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="87" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C87" s="2" t="s">
         <v>75</v>
       </c>
@@ -1716,12 +1718,12 @@
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
     </row>
-    <row r="88" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B88" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="89" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C89" s="2" t="s">
         <v>77</v>
       </c>
@@ -1729,7 +1731,7 @@
       <c r="F89" s="7"/>
       <c r="G89" s="7"/>
     </row>
-    <row r="90" spans="1:7" ht="30" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="29" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="C90" s="2" t="s">
         <v>78</v>
       </c>
@@ -1737,7 +1739,7 @@
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E91" s="1" t="s">
         <v>79</v>
       </c>
@@ -1748,7 +1750,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>80</v>
       </c>
@@ -1765,7 +1767,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="93" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B93" s="1" t="s">
         <v>81</v>
       </c>
@@ -1773,7 +1775,7 @@
       <c r="F93" s="7"/>
       <c r="G93" s="7"/>
     </row>
-    <row r="94" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B94" s="1" t="s">
         <v>82</v>
       </c>
@@ -1781,7 +1783,7 @@
       <c r="F94" s="7"/>
       <c r="G94" s="7"/>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>83</v>
       </c>
@@ -1798,7 +1800,7 @@
         <v>O</v>
       </c>
     </row>
-    <row r="96" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B96" s="1" t="s">
         <v>84</v>
       </c>
@@ -1806,7 +1808,7 @@
       <c r="F96" s="7"/>
       <c r="G96" s="7"/>
     </row>
-    <row r="97" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="B97" s="1" t="s">
         <v>85</v>
       </c>
@@ -1890,14 +1892,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -1905,7 +1907,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>88</v>
       </c>
@@ -1913,7 +1915,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>90</v>
       </c>

</xml_diff>